<commit_message>
Render poster's map panels
</commit_message>
<xml_diff>
--- a/D_Misc/PanelLayoutPlan.xlsx
+++ b/D_Misc/PanelLayoutPlan.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/s8/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/s8/Documents/Coding/road_trips/D_Misc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED64E259-9111-534B-BB71-07DDAACECB23}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7CF8653-E1CA-8D40-A1F6-F0B26297F750}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="15300" yWindow="500" windowWidth="17040" windowHeight="13220" xr2:uid="{1679F9CE-3519-4E43-973F-DB3FE1E69E32}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -77,7 +77,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -145,17 +145,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="166" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="166" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="166" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="166" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -473,7 +473,7 @@
   <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -537,22 +537,22 @@
       </c>
       <c r="B3" s="10">
         <f>E3*1.623</f>
-        <v>29.051699999999997</v>
+        <v>28.4025</v>
       </c>
       <c r="C3" s="11">
         <v>0.5</v>
       </c>
       <c r="D3" s="10">
         <f>C3+B3</f>
-        <v>29.551699999999997</v>
+        <v>28.9025</v>
       </c>
       <c r="E3" s="10">
         <f>G3-F3</f>
-        <v>17.899999999999999</v>
+        <v>17.5</v>
       </c>
       <c r="F3" s="13">
-        <f>G4+0.1</f>
-        <v>5.6</v>
+        <f>G4+0.5</f>
+        <v>6</v>
       </c>
       <c r="G3" s="11">
         <v>23.5</v>
@@ -564,11 +564,11 @@
       </c>
       <c r="B4" s="10">
         <f>D4-C4</f>
-        <v>29.9</v>
+        <v>26.384999999999998</v>
       </c>
       <c r="C4" s="13">
-        <f>G2+0.1</f>
-        <v>5.6</v>
+        <f>D2+0.5</f>
+        <v>9.1150000000000002</v>
       </c>
       <c r="D4" s="11">
         <v>35.5</v>
@@ -591,22 +591,22 @@
       </c>
       <c r="B5" s="10">
         <f>D5-C5</f>
-        <v>5.8483000000000018</v>
+        <v>6.0975000000000001</v>
       </c>
       <c r="C5" s="13">
-        <f>D3+0.1</f>
-        <v>29.651699999999998</v>
+        <f>D3+0.5</f>
+        <v>29.4025</v>
       </c>
       <c r="D5" s="11">
         <v>35.5</v>
       </c>
       <c r="E5" s="10">
         <f>E3</f>
-        <v>17.899999999999999</v>
+        <v>17.5</v>
       </c>
       <c r="F5" s="13">
         <f>F3</f>
-        <v>5.6</v>
+        <v>6</v>
       </c>
       <c r="G5" s="11">
         <v>23.5</v>

</xml_diff>